<commit_message>
add new handel barr
</commit_message>
<xml_diff>
--- a/uploads/leave.xlsx
+++ b/uploads/leave.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>aashish@ashmar.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aanand </t>
+  </si>
+  <si>
+    <t>anand@monetnetworks.com</t>
   </si>
 </sst>
 </file>
@@ -376,7 +382,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,9 +421,23 @@
       <c r="D2">
         <v>3</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>

</xml_diff>